<commit_message>
milestone 2 - submission 1
</commit_message>
<xml_diff>
--- a/docs/bug-report.xlsx
+++ b/docs/bug-report.xlsx
@@ -11,24 +11,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment authorId="0" ref="D4">
-      <text>
-        <t xml:space="preserve">(P0 = crash bug, P1 = game stopping but not crash, P2 = not working as expected, P3 = annoying, P4 = nice to have, P5 = future release)
-	-Nic Ung</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="61">
   <si>
     <t>Bug List</t>
   </si>
@@ -69,7 +53,7 @@
     <t>P3</t>
   </si>
   <si>
-    <t>in-progress</t>
+    <t>resolved</t>
   </si>
   <si>
     <t xml:space="preserve">Multiple attack while holding attack key. </t>
@@ -90,9 +74,6 @@
     <t>P2</t>
   </si>
   <si>
-    <t>open</t>
-  </si>
-  <si>
     <t>Siddh</t>
   </si>
   <si>
@@ -108,6 +89,84 @@
     <t>Move player 1 to touch the Left Wall, Move player 2 to touch player 1, Have player 1 try to move right and then have player 2 try to move right. Player 2 will not be able to move until player 1 releases the key.</t>
   </si>
   <si>
+    <t>Roy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Player get stuck when jumping into one another </t>
+  </si>
+  <si>
+    <t>Players should stop when they collide with the other player in the air</t>
+  </si>
+  <si>
+    <t>the Player jumping get's stuck in the air, and both players become stuc</t>
+  </si>
+  <si>
+    <t>Move Player 1 close to Player 2, and then jump towards them, Player one will be unable to move in any direction</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>Players can move during loading animation</t>
+  </si>
+  <si>
+    <t>During the loading animation before both players are at full sized and have not yet touched the ground. The players should not be able to move</t>
+  </si>
+  <si>
+    <t>Players can currently press movement keys to move during the loading animation, which looks weird</t>
+  </si>
+  <si>
+    <t>Starting a fresh game doesn't have this bug, due to there being no interpolation loading. First, defeat the enemy player and press Enter to start a new round. You'll notice players being interpolated from the edge of the screen, you can press movement keys to move your character during this time</t>
+  </si>
+  <si>
+    <t>P4</t>
+  </si>
+  <si>
+    <t>game crashes after a few minutes</t>
+  </si>
+  <si>
+    <t>Game shouldn't cause any performance issues</t>
+  </si>
+  <si>
+    <t>When the game is ran, pc experiences performance issues after a while</t>
+  </si>
+  <si>
+    <t>Leave the game on in the background for a few minutes, pc should start slowing down with the game crashing after a while</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>Armaan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">when restarting the game, the last frame of the last fight will shows </t>
+  </si>
+  <si>
+    <t>The screen should be clear with both characters coming in from the two sides</t>
+  </si>
+  <si>
+    <t>The two characters will be in the positions that they were in at the end of the last fight</t>
+  </si>
+  <si>
+    <t>Restart the battle after a battle ends and the last frame will show up for a split second</t>
+  </si>
+  <si>
+    <t>Jenny/Roy</t>
+  </si>
+  <si>
+    <t>Players can drag each other in the screen if you try to move out of the camera area</t>
+  </si>
+  <si>
+    <t>When both players are at their respective camera edge bounds, and they try to move away from one another, the camera should stay in place and prevent both players from moving</t>
+  </si>
+  <si>
+    <t>When both players are at their respective camera edge bounds, and one player tries moving outside of camera area, the screen follows the moving player and drags the other player with it</t>
+  </si>
+  <si>
+    <t>Move both players to the edge of the game screen. Try to move the player on the right towards the right. You should see the camera move, dragging the player on the left.</t>
+  </si>
+  <si>
     <t>Severity</t>
   </si>
   <si>
@@ -120,9 +179,6 @@
     <t>crash bug; game crashes and is unrecoverable</t>
   </si>
   <si>
-    <t>P1</t>
-  </si>
-  <si>
     <t>game stopping bug, but no crash; cannot keep playing</t>
   </si>
   <si>
@@ -130,9 +186,6 @@
   </si>
   <si>
     <t>annoying, could ship but loss of marks</t>
-  </si>
-  <si>
-    <t>P4</t>
   </si>
   <si>
     <t>annoying or limiting, but could be shipped as-is</t>
@@ -148,8 +201,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="165" formatCode="yyyy/mm/dd"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -216,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -233,16 +287,25 @@
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
+      <alignment readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -475,8 +538,8 @@
     <col customWidth="1" min="5" max="5" width="32.75"/>
     <col customWidth="1" min="6" max="6" width="14.5"/>
     <col customWidth="1" min="7" max="7" width="22.13"/>
-    <col customWidth="1" min="8" max="8" width="19.88"/>
-    <col customWidth="1" min="9" max="9" width="19.75"/>
+    <col customWidth="1" min="8" max="8" width="23.25"/>
+    <col customWidth="1" min="9" max="9" width="23.63"/>
     <col customWidth="1" min="10" max="10" width="48.75"/>
   </cols>
   <sheetData>
@@ -545,270 +608,240 @@
       <c r="G4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="5">
+    <row r="5" ht="14.25" customHeight="1"/>
+    <row r="6" ht="14.25" customHeight="1"/>
+    <row r="7" ht="14.25" customHeight="1"/>
+    <row r="8" ht="14.25" customHeight="1"/>
+    <row r="9" ht="14.25" customHeight="1"/>
+    <row r="10" ht="14.25" customHeight="1">
+      <c r="A10" s="5">
         <v>2.0</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B10" s="6">
         <v>45578.0</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="G10" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="H10" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="I10" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="J10" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="8" t="s">
+    </row>
+    <row r="11" ht="14.25" customHeight="1"/>
+    <row r="12" ht="14.25" customHeight="1"/>
+    <row r="13" ht="14.25" customHeight="1"/>
+    <row r="14" ht="14.25" customHeight="1">
+      <c r="A14" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="B14" s="6">
+        <v>45214.0</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" ht="14.25" customHeight="1">
-      <c r="G6" s="2"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-    </row>
-    <row r="7" ht="14.25" customHeight="1">
-      <c r="G7" s="2"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-    </row>
-    <row r="8" ht="14.25" customHeight="1">
-      <c r="G8" s="2"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-    </row>
-    <row r="9" ht="14.25" customHeight="1">
-      <c r="G9" s="2"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-    </row>
-    <row r="10" ht="14.25" customHeight="1">
-      <c r="G10" s="2"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-    </row>
-    <row r="11" ht="14.25" customHeight="1">
-      <c r="G11" s="2"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-    </row>
-    <row r="12" ht="14.25" customHeight="1">
-      <c r="G12" s="2"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-    </row>
-    <row r="13" ht="14.25" customHeight="1">
-      <c r="G13" s="2"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-    </row>
-    <row r="14" ht="14.25" customHeight="1">
-      <c r="G14" s="2"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-    </row>
-    <row r="15" ht="14.25" customHeight="1">
-      <c r="G15" s="2"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-    </row>
-    <row r="16" ht="14.25" customHeight="1">
-      <c r="G16" s="2"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-    </row>
-    <row r="17" ht="14.25" customHeight="1">
-      <c r="G17" s="2"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-    </row>
+      <c r="D14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" ht="14.25" customHeight="1"/>
+    <row r="16" ht="14.25" customHeight="1"/>
+    <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1">
-      <c r="G18" s="2"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-    </row>
-    <row r="19" ht="14.25" customHeight="1">
-      <c r="G19" s="2"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-    </row>
-    <row r="20" ht="14.25" customHeight="1">
-      <c r="G20" s="2"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-    </row>
-    <row r="21" ht="14.25" customHeight="1">
-      <c r="G21" s="2"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-    </row>
-    <row r="22" ht="14.25" customHeight="1">
-      <c r="G22" s="2"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-    </row>
-    <row r="23" ht="14.25" customHeight="1">
-      <c r="G23" s="2"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-    </row>
+      <c r="A18" s="5">
+        <v>4.0</v>
+      </c>
+      <c r="B18" s="10">
+        <v>45600.0</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" ht="14.25" customHeight="1"/>
+    <row r="20" ht="14.25" customHeight="1"/>
+    <row r="21" ht="14.25" customHeight="1"/>
+    <row r="22" ht="14.25" customHeight="1"/>
+    <row r="23" ht="14.25" customHeight="1"/>
     <row r="24" ht="14.25" customHeight="1">
-      <c r="G24" s="2"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-    </row>
-    <row r="25" ht="14.25" customHeight="1">
-      <c r="G25" s="2"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-    </row>
-    <row r="26" ht="14.25" customHeight="1">
-      <c r="G26" s="2"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-    </row>
-    <row r="27" ht="14.25" customHeight="1">
-      <c r="G27" s="2"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-    </row>
-    <row r="28" ht="14.25" customHeight="1">
-      <c r="G28" s="2"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-    </row>
+      <c r="A24" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="B24" s="10">
+        <v>45600.0</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J24" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" ht="14.25" customHeight="1"/>
+    <row r="26" ht="14.25" customHeight="1"/>
+    <row r="27" ht="14.25" customHeight="1"/>
+    <row r="28" ht="14.25" customHeight="1"/>
     <row r="29" ht="14.25" customHeight="1">
-      <c r="G29" s="2"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-    </row>
-    <row r="30" ht="14.25" customHeight="1">
-      <c r="G30" s="2"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-    </row>
-    <row r="31" ht="14.25" customHeight="1">
-      <c r="G31" s="2"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-    </row>
-    <row r="32" ht="14.25" customHeight="1">
-      <c r="G32" s="2"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
-    </row>
-    <row r="33" ht="14.25" customHeight="1">
-      <c r="G33" s="2"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-    </row>
+      <c r="A29" s="11">
+        <v>6.0</v>
+      </c>
+      <c r="B29" s="10">
+        <v>45600.0</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H29" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="I29" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="J29" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" ht="14.25" customHeight="1"/>
+    <row r="31" ht="14.25" customHeight="1"/>
+    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1">
-      <c r="G34" s="2"/>
-      <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
-    </row>
-    <row r="35" ht="14.25" customHeight="1">
-      <c r="G35" s="2"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-    </row>
-    <row r="36" ht="14.25" customHeight="1">
-      <c r="G36" s="2"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
-    </row>
-    <row r="37" ht="14.25" customHeight="1">
-      <c r="G37" s="2"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
-    </row>
-    <row r="38" ht="14.25" customHeight="1">
-      <c r="G38" s="2"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
-    </row>
-    <row r="39" ht="14.25" customHeight="1">
-      <c r="G39" s="2"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
-    </row>
-    <row r="40" ht="14.25" customHeight="1">
-      <c r="G40" s="2"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
-    </row>
-    <row r="41" ht="14.25" customHeight="1">
-      <c r="G41" s="2"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
-      <c r="J41" s="3"/>
-    </row>
-    <row r="42" ht="14.25" customHeight="1">
-      <c r="G42" s="2"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
-    </row>
+      <c r="A34" s="11">
+        <v>7.0</v>
+      </c>
+      <c r="B34" s="10">
+        <v>45600.0</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H34" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I34" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="J34" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" ht="14.25" customHeight="1"/>
+    <row r="36" ht="14.25" customHeight="1"/>
+    <row r="37" ht="14.25" customHeight="1"/>
+    <row r="38" ht="14.25" customHeight="1"/>
+    <row r="39" ht="14.25" customHeight="1"/>
+    <row r="40" ht="14.25" customHeight="1"/>
+    <row r="41" ht="14.25" customHeight="1"/>
+    <row r="42" ht="14.25" customHeight="1"/>
     <row r="43" ht="14.25" customHeight="1">
       <c r="G43" s="2"/>
       <c r="H43" s="3"/>
@@ -6558,14 +6591,83 @@
       <c r="J1000" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="71">
+    <mergeCell ref="H18:H23"/>
+    <mergeCell ref="I18:I23"/>
+    <mergeCell ref="J18:J23"/>
+    <mergeCell ref="A18:A23"/>
+    <mergeCell ref="B18:B23"/>
+    <mergeCell ref="C18:C23"/>
+    <mergeCell ref="D18:D23"/>
+    <mergeCell ref="E18:E23"/>
+    <mergeCell ref="F18:F23"/>
+    <mergeCell ref="G18:G23"/>
+    <mergeCell ref="H24:H28"/>
+    <mergeCell ref="I24:I28"/>
+    <mergeCell ref="J24:J28"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="B24:B28"/>
+    <mergeCell ref="C24:C28"/>
+    <mergeCell ref="D24:D28"/>
+    <mergeCell ref="E24:E28"/>
+    <mergeCell ref="F24:F28"/>
+    <mergeCell ref="G24:G28"/>
+    <mergeCell ref="H29:H33"/>
+    <mergeCell ref="I29:I33"/>
+    <mergeCell ref="J29:J33"/>
+    <mergeCell ref="A29:A33"/>
+    <mergeCell ref="B29:B33"/>
+    <mergeCell ref="C29:C33"/>
+    <mergeCell ref="D29:D33"/>
+    <mergeCell ref="E29:E33"/>
+    <mergeCell ref="F29:F33"/>
+    <mergeCell ref="G29:G33"/>
+    <mergeCell ref="J4:J9"/>
+    <mergeCell ref="I4:I9"/>
+    <mergeCell ref="H4:H9"/>
+    <mergeCell ref="G4:G9"/>
     <mergeCell ref="A1:J1"/>
+    <mergeCell ref="F4:F9"/>
+    <mergeCell ref="E4:E9"/>
+    <mergeCell ref="D4:D9"/>
+    <mergeCell ref="C4:C9"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="H10:H13"/>
+    <mergeCell ref="I10:I13"/>
+    <mergeCell ref="J10:J13"/>
+    <mergeCell ref="H14:H17"/>
+    <mergeCell ref="I14:I17"/>
+    <mergeCell ref="J14:J17"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="F10:F13"/>
+    <mergeCell ref="G10:G13"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="E14:E17"/>
+    <mergeCell ref="F14:F17"/>
+    <mergeCell ref="G14:G17"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="D14:D17"/>
+    <mergeCell ref="A34:A38"/>
+    <mergeCell ref="I34:I42"/>
+    <mergeCell ref="J34:J42"/>
+    <mergeCell ref="B34:B42"/>
+    <mergeCell ref="C34:C42"/>
+    <mergeCell ref="D34:D42"/>
+    <mergeCell ref="E34:E42"/>
+    <mergeCell ref="F34:F42"/>
+    <mergeCell ref="G34:G42"/>
+    <mergeCell ref="H34:H42"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6583,59 +6685,59 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>27</v>
+      <c r="A1" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>29</v>
+      <c r="A2" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>31</v>
+      <c r="A3" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>32</v>
+      <c r="B4" s="12" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>33</v>
+      <c r="B5" s="12" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" s="9" t="s">
+      <c r="A6" s="13" t="s">
         <v>35</v>
       </c>
+      <c r="B6" s="12" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>37</v>
+      <c r="A7" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1"/>

</xml_diff>